<commit_message>
More test cases for registration form added
</commit_message>
<xml_diff>
--- a/TestCases/Test-Cases-Registration-Ilvie.xlsx
+++ b/TestCases/Test-Cases-Registration-Ilvie.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="99">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -939,37 +939,6 @@
     <r>
       <t>1. Navigate to http://stage.telerikacademy.com/
 2. Click "Registration"/"Регистрация" button
-3. Enter invalid</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> e-mail address</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that does not contain '.'  in the domain part or '@' after the
-local part 
-4. Click "Registration"/"Регистрация" button </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1. Navigate to http://stage.telerikacademy.com/
-2. Click "Registration"/"Регистрация" button
 3. Enter</t>
     </r>
     <r>
@@ -1053,6 +1022,346 @@
 6. Accept the license agreement
 7. Click "Registration"/"Регистрация" button</t>
     </r>
+  </si>
+  <si>
+    <t>Verifiy the user is navigated to http://stage.telerikacademy.com/Users/Auth/Registration without errors.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Navigate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+</t>
+    </r>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1. Verifiy the link with Terms and Conditions is not broken
+2. Ensure the user is navigated to new web page with pdf document</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>1. Verifiy that all six text fields are present on the page
+2. Verifiy that a checkbox is present on the page
+3. Verifiy that a link with rules is present on the page
+4.  Verifiy that the registration button is present on the page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Verifiy the lebels for all six text fields are present on the page
+2. Verifiy the lebel for checkbox is present on the page
+</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Navigate to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+3. Click to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>link</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> "Свалете правилата и условията" </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Navigate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Navigate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Navigate to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+3. Enter invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e-mail address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that does not contain '.'  in the domain part
+4. Click "Registration"/"Регистрация" button </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Navigate to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+3. Enter invalid</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> e-mail address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that does not contain '@' after the local part 
+4. Click "Registration"/"Регистрация" button </t>
+    </r>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Navigate to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+3. Enter valid values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">all text fields </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+4. Accept the license agreement
+5. Click "Registration"/"Регистрация" button
+6. Click Logout buttot
+7.  Click "Registration"/"Регистрация" button
+8. Enter the samе </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>username</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as in 3.
+9. Accept the license agreement
+10. Click "Registration"/"Регистрация" button</t>
+    </r>
+  </si>
+  <si>
+    <t>The following error should be displayed "Потребителското име вече е заето."</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Navigate to http://stage.telerikacademy.com/
+2. Click "Registration"/"Регистрация" button
+3. Enter valid values for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">all text fields </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+4. Accept the license agreement
+5. Click "Registration"/"Регистрация" button
+6. Click Logout buttot
+7.  Click "Registration"/"Регистрация" button
+8. Enter the samе </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>e-mail address</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> as in 3.
+9. Accept the license agreement
+10. Click "Registration"/"Регистрация" button</t>
+    </r>
+  </si>
+  <si>
+    <t>The following error should be displayed "Този емейл адрес вече се използва от друг потребител."</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1558,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1291,6 +1600,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1588,10 +1900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:K27"/>
+  <dimension ref="B1:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1600,9 +1912,9 @@
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="20.140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="54.42578125" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" customWidth="1"/>
-    <col min="8" max="8" width="25" customWidth="1"/>
+    <col min="6" max="6" width="59" customWidth="1"/>
+    <col min="7" max="7" width="58.140625" customWidth="1"/>
+    <col min="8" max="8" width="55.85546875" customWidth="1"/>
     <col min="9" max="9" width="47.28515625" customWidth="1"/>
     <col min="10" max="10" width="28.5703125" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
@@ -1636,13 +1948,13 @@
         <v>7</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="93.75" customHeight="1">
+    <row r="3" spans="2:11" ht="60" customHeight="1">
       <c r="B3" s="6">
         <v>1</v>
       </c>
@@ -1656,10 +1968,10 @@
         <v>11</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>12</v>
+        <v>77</v>
       </c>
       <c r="H3" s="12"/>
       <c r="I3" s="9"/>
@@ -1668,7 +1980,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="2:11" ht="110.25" customHeight="1">
+    <row r="4" spans="2:11" ht="89.25" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>14</v>
       </c>
@@ -1682,10 +1994,10 @@
         <v>11</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="H4" s="12"/>
       <c r="I4" s="9"/>
@@ -1694,12 +2006,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="72.75" customHeight="1">
+    <row r="5" spans="2:11" ht="59.25" customHeight="1">
       <c r="B5" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>9</v>
+        <v>83</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>10</v>
@@ -1708,10 +2020,10 @@
         <v>11</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>40</v>
+        <v>85</v>
       </c>
       <c r="H5" s="12"/>
       <c r="I5" s="9"/>
@@ -1720,7 +2032,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="92.25" customHeight="1">
+    <row r="6" spans="2:11" ht="93.75" customHeight="1">
       <c r="B6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1734,10 +2046,10 @@
         <v>11</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
       <c r="H6" s="12"/>
       <c r="I6" s="9"/>
@@ -1746,7 +2058,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="2:11" ht="114.75" customHeight="1">
+    <row r="7" spans="2:11" ht="162" customHeight="1">
       <c r="B7" s="6" t="s">
         <v>21</v>
       </c>
@@ -1759,11 +2071,11 @@
       <c r="E7" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>44</v>
+      <c r="F7" s="15" t="s">
+        <v>93</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="H7" s="12"/>
       <c r="I7" s="9"/>
@@ -1772,7 +2084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="2:11" ht="119.25" customHeight="1">
+    <row r="8" spans="2:11" ht="162" customHeight="1">
       <c r="B8" s="6" t="s">
         <v>24</v>
       </c>
@@ -1785,11 +2097,11 @@
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>47</v>
+      <c r="F8" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>45</v>
+        <v>96</v>
       </c>
       <c r="H8" s="12"/>
       <c r="I8" s="9"/>
@@ -1798,7 +2110,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:11" ht="98.25" customHeight="1">
+    <row r="9" spans="2:11" ht="110.25" customHeight="1">
       <c r="B9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1812,10 +2124,10 @@
         <v>11</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>45</v>
+        <v>15</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="9"/>
@@ -1824,7 +2136,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="124.5" customHeight="1">
+    <row r="10" spans="2:11" ht="72.75" customHeight="1">
       <c r="B10" s="6" t="s">
         <v>29</v>
       </c>
@@ -1837,11 +2149,11 @@
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>77</v>
+      <c r="F10" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="H10" s="12"/>
       <c r="I10" s="9"/>
@@ -1850,7 +2162,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="2:11" ht="95.25" customHeight="1">
+    <row r="11" spans="2:11" ht="92.25" customHeight="1">
       <c r="B11" s="6" t="s">
         <v>32</v>
       </c>
@@ -1864,18 +2176,19 @@
         <v>11</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="H11" s="12"/>
       <c r="I11" s="9"/>
-      <c r="J11" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="2:11" ht="82.5" customHeight="1">
+      <c r="J11" s="9"/>
+      <c r="K11" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="114.75" customHeight="1">
       <c r="B12" s="6" t="s">
         <v>35</v>
       </c>
@@ -1889,10 +2202,10 @@
         <v>11</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="H12" s="12"/>
       <c r="I12" s="9"/>
@@ -1901,7 +2214,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="107.25" customHeight="1">
+    <row r="13" spans="2:11" ht="119.25" customHeight="1">
       <c r="B13" s="6" t="s">
         <v>38</v>
       </c>
@@ -1915,10 +2228,10 @@
         <v>11</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="H13" s="12"/>
       <c r="I13" s="9"/>
@@ -1927,7 +2240,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="2:11" ht="106.5" customHeight="1">
+    <row r="14" spans="2:11" ht="98.25" customHeight="1">
       <c r="B14" s="6" t="s">
         <v>41</v>
       </c>
@@ -1941,10 +2254,10 @@
         <v>11</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>33</v>
+        <v>49</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="9"/>
@@ -1953,7 +2266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="102.75" customHeight="1">
+    <row r="15" spans="2:11" ht="124.5" customHeight="1">
       <c r="B15" s="6" t="s">
         <v>43</v>
       </c>
@@ -1966,11 +2279,11 @@
       <c r="E15" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>54</v>
+      <c r="F15" s="14" t="s">
+        <v>76</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="9"/>
@@ -1979,7 +2292,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="116.25" customHeight="1">
+    <row r="16" spans="2:11" ht="95.25" customHeight="1">
       <c r="B16" s="6" t="s">
         <v>46</v>
       </c>
@@ -1993,19 +2306,18 @@
         <v>11</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>56</v>
+        <v>30</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="H16" s="12"/>
       <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="110.25" customHeight="1">
+      <c r="J16" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="82.5" customHeight="1">
       <c r="B17" s="6" t="s">
         <v>48</v>
       </c>
@@ -2019,10 +2331,10 @@
         <v>11</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="H17" s="12"/>
       <c r="I17" s="9"/>
@@ -2031,7 +2343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="106.5" customHeight="1">
+    <row r="18" spans="2:11" ht="107.25" customHeight="1">
       <c r="B18" s="6" t="s">
         <v>50</v>
       </c>
@@ -2045,10 +2357,10 @@
         <v>11</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>60</v>
+        <v>19</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H18" s="12"/>
       <c r="I18" s="9"/>
@@ -2057,7 +2369,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="136.5" customHeight="1">
+    <row r="19" spans="2:11" ht="106.5" customHeight="1">
       <c r="B19" s="6" t="s">
         <v>53</v>
       </c>
@@ -2071,10 +2383,10 @@
         <v>11</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="H19" s="12"/>
       <c r="I19" s="9"/>
@@ -2083,7 +2395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="102" customHeight="1">
+    <row r="20" spans="2:11" ht="102.75" customHeight="1">
       <c r="B20" s="6" t="s">
         <v>55</v>
       </c>
@@ -2097,10 +2409,10 @@
         <v>11</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>36</v>
+        <v>54</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H20" s="12"/>
       <c r="I20" s="9"/>
@@ -2109,7 +2421,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:11" ht="97.5" customHeight="1">
+    <row r="21" spans="2:11" ht="116.25" customHeight="1">
       <c r="B21" s="6" t="s">
         <v>57</v>
       </c>
@@ -2123,10 +2435,10 @@
         <v>11</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H21" s="12"/>
       <c r="I21" s="9"/>
@@ -2135,7 +2447,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="2:11" ht="122.25" customHeight="1">
+    <row r="22" spans="2:11" ht="110.25" customHeight="1">
       <c r="B22" s="6" t="s">
         <v>59</v>
       </c>
@@ -2149,10 +2461,10 @@
         <v>11</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="9"/>
@@ -2161,7 +2473,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="2:11" ht="107.25" customHeight="1">
+    <row r="23" spans="2:11" ht="106.5" customHeight="1">
       <c r="B23" s="6" t="s">
         <v>61</v>
       </c>
@@ -2175,10 +2487,10 @@
         <v>11</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H23" s="12"/>
       <c r="I23" s="9"/>
@@ -2187,7 +2499,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="2:11" ht="109.5" customHeight="1">
+    <row r="24" spans="2:11" ht="136.5" customHeight="1">
       <c r="B24" s="6" t="s">
         <v>63</v>
       </c>
@@ -2201,10 +2513,10 @@
         <v>11</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>73</v>
+        <v>22</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="9"/>
@@ -2213,7 +2525,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="2:11" ht="123" customHeight="1">
+    <row r="25" spans="2:11" ht="102" customHeight="1">
       <c r="B25" s="6" t="s">
         <v>65</v>
       </c>
@@ -2227,21 +2539,19 @@
         <v>11</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>74</v>
+        <v>36</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="H25" s="12"/>
-      <c r="I25" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J25" s="13"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
       <c r="K25" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="2:11" ht="95.25" customHeight="1">
+    <row r="26" spans="2:11" ht="97.5" customHeight="1">
       <c r="B26" s="6" t="s">
         <v>67</v>
       </c>
@@ -2255,19 +2565,19 @@
         <v>11</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="H26" s="12"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
+      <c r="I26" s="9"/>
+      <c r="J26" s="9"/>
       <c r="K26" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="2:11" ht="107.25" customHeight="1">
+    <row r="27" spans="2:11" ht="122.25" customHeight="1">
       <c r="B27" s="6" t="s">
         <v>69</v>
       </c>
@@ -2281,10 +2591,10 @@
         <v>11</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="9"/>
@@ -2293,12 +2603,199 @@
         <v>13</v>
       </c>
     </row>
+    <row r="28" spans="2:11" ht="107.25" customHeight="1">
+      <c r="B28" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="12"/>
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="2:11" ht="109.5" customHeight="1">
+      <c r="B29" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H29" s="12"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="2:11" ht="123" customHeight="1">
+      <c r="B30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H30" s="12"/>
+      <c r="I30" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J30" s="13"/>
+      <c r="K30" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="2:11" ht="94.5" customHeight="1">
+      <c r="B31" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" ht="95.25" customHeight="1">
+      <c r="B32" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H32" s="12"/>
+      <c r="I32" s="13"/>
+      <c r="J32" s="13"/>
+      <c r="K32" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" ht="107.25" customHeight="1">
+      <c r="B33" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H33" s="12"/>
+      <c r="I33" s="9"/>
+      <c r="J33" s="9"/>
+      <c r="K33" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" ht="79.5" customHeight="1">
+      <c r="B34" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C34" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9"/>
+      <c r="K34" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I25" r:id="rId1"/>
+    <hyperlink ref="I31" r:id="rId1"/>
+    <hyperlink ref="I30" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>